<commit_message>
'Update: Previsão Jan-Mar 2023'
</commit_message>
<xml_diff>
--- a/datasets_cestas/accb_custo_total_ilheus.xlsx
+++ b/datasets_cestas/accb_custo_total_ilheus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\NotebooksMateriais\previsao_cestas\datasets_cestas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Dropbox\PythonNotebooks\previsao_cestas\datasets_cestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCB7E8A-FC3D-4C87-8ACF-0BA19E80A47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F049CE4B-93D7-4F0F-B686-03A3D79EBF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,13 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,7 +290,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B217" sqref="B217"/>
+      <selection activeCell="J215" sqref="J215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1885,364 +1883,368 @@
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="3">
+      <c r="A199" s="2">
         <v>44348</v>
       </c>
-      <c r="B199" s="4">
+      <c r="B199" s="1">
         <v>426.7</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="3">
+      <c r="A200" s="2">
         <v>44378</v>
       </c>
-      <c r="B200" s="4">
+      <c r="B200" s="1">
         <v>420.44</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="5">
+      <c r="A201" s="3">
         <v>44409</v>
       </c>
-      <c r="B201" s="4">
+      <c r="B201" s="1">
         <v>428.43</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="5">
+      <c r="A202" s="3">
         <v>44440</v>
       </c>
-      <c r="B202" s="4">
+      <c r="B202" s="1">
         <v>443.13</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="5">
+      <c r="A203" s="3">
         <v>44470</v>
       </c>
-      <c r="B203" s="4">
+      <c r="B203" s="1">
         <v>482.65</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="5">
+      <c r="A204" s="3">
         <v>44501</v>
       </c>
-      <c r="B204" s="4">
+      <c r="B204" s="1">
         <v>478.52</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="5">
+      <c r="A205" s="3">
         <v>44531</v>
       </c>
-      <c r="B205" s="4">
+      <c r="B205" s="1">
         <v>482.87</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="5">
+      <c r="A206" s="3">
         <v>44562</v>
       </c>
-      <c r="B206" s="4">
+      <c r="B206" s="1">
         <v>540.42999999999995</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="5">
+      <c r="A207" s="3">
         <v>44593</v>
       </c>
-      <c r="B207" s="4">
+      <c r="B207" s="1">
         <v>527.59</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="5">
+      <c r="A208" s="3">
         <v>44621</v>
       </c>
-      <c r="B208" s="4">
+      <c r="B208" s="1">
         <v>534.26</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="5">
+      <c r="A209" s="3">
         <v>44652</v>
       </c>
-      <c r="B209" s="4">
+      <c r="B209" s="1">
         <v>558.79999999999995</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="5">
+      <c r="A210" s="3">
         <v>44682</v>
       </c>
-      <c r="B210" s="4">
+      <c r="B210" s="1">
         <v>534.01</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="5">
+      <c r="A211" s="3">
         <v>44713</v>
       </c>
-      <c r="B211" s="4">
+      <c r="B211" s="1">
         <v>537.30999999999995</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="5">
+      <c r="A212" s="3">
         <v>44743</v>
       </c>
-      <c r="B212" s="4">
+      <c r="B212" s="1">
         <v>538.27</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="5">
+      <c r="A213" s="3">
         <v>44774</v>
       </c>
-      <c r="B213" s="4">
+      <c r="B213" s="1">
         <v>516.04</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="5">
+      <c r="A214" s="3">
         <v>44805</v>
       </c>
-      <c r="B214" s="4">
+      <c r="B214" s="1">
         <v>520.57000000000005</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A215" s="5">
+      <c r="A215" s="3">
         <v>44835</v>
       </c>
-      <c r="B215" s="4">
+      <c r="B215" s="1">
         <v>522.13</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A216" s="5">
+      <c r="A216" s="3">
         <v>44866</v>
       </c>
-      <c r="B216" s="4">
+      <c r="B216" s="1">
         <v>522.67999999999995</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="5"/>
-      <c r="B217" s="4"/>
+      <c r="A217" s="3">
+        <v>44896</v>
+      </c>
+      <c r="B217" s="1">
+        <v>536.80999999999995</v>
+      </c>
     </row>
     <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="5"/>
-      <c r="B218" s="4"/>
+      <c r="A218" s="3"/>
+      <c r="B218" s="1"/>
     </row>
     <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="5"/>
-      <c r="B219" s="4"/>
+      <c r="A219" s="3"/>
+      <c r="B219" s="1"/>
     </row>
     <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="5"/>
-      <c r="B220" s="4"/>
+      <c r="A220" s="3"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="5"/>
-      <c r="B221" s="4"/>
+      <c r="A221" s="3"/>
+      <c r="B221" s="1"/>
     </row>
     <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="5"/>
-      <c r="B222" s="4"/>
+      <c r="A222" s="3"/>
+      <c r="B222" s="1"/>
     </row>
     <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A223" s="5"/>
-      <c r="B223" s="4"/>
+      <c r="A223" s="3"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="5"/>
-      <c r="B224" s="4"/>
+      <c r="A224" s="3"/>
+      <c r="B224" s="1"/>
     </row>
     <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="5"/>
-      <c r="B225" s="4"/>
+      <c r="A225" s="3"/>
+      <c r="B225" s="1"/>
     </row>
     <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="5"/>
-      <c r="B226" s="4"/>
+      <c r="A226" s="3"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="5"/>
-      <c r="B227" s="4"/>
+      <c r="A227" s="3"/>
+      <c r="B227" s="1"/>
     </row>
     <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="5"/>
-      <c r="B228" s="4"/>
+      <c r="A228" s="3"/>
+      <c r="B228" s="1"/>
     </row>
     <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="5"/>
-      <c r="B229" s="4"/>
+      <c r="A229" s="3"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A230" s="5"/>
-      <c r="B230" s="4"/>
+      <c r="A230" s="3"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="5"/>
-      <c r="B231" s="4"/>
+      <c r="A231" s="3"/>
+      <c r="B231" s="1"/>
     </row>
     <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A232" s="5"/>
-      <c r="B232" s="4"/>
+      <c r="A232" s="3"/>
+      <c r="B232" s="1"/>
     </row>
     <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A233" s="5"/>
-      <c r="B233" s="4"/>
+      <c r="A233" s="3"/>
+      <c r="B233" s="1"/>
     </row>
     <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="5"/>
-      <c r="B234" s="4"/>
+      <c r="A234" s="3"/>
+      <c r="B234" s="1"/>
     </row>
     <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="5"/>
-      <c r="B235" s="4"/>
+      <c r="A235" s="3"/>
+      <c r="B235" s="1"/>
     </row>
     <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="5"/>
-      <c r="B236" s="4"/>
+      <c r="A236" s="3"/>
+      <c r="B236" s="1"/>
     </row>
     <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A237" s="5"/>
-      <c r="B237" s="4"/>
+      <c r="A237" s="3"/>
+      <c r="B237" s="1"/>
     </row>
     <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A238" s="5"/>
-      <c r="B238" s="4"/>
+      <c r="A238" s="3"/>
+      <c r="B238" s="1"/>
     </row>
     <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A239" s="5"/>
-      <c r="B239" s="4"/>
+      <c r="A239" s="3"/>
+      <c r="B239" s="1"/>
     </row>
     <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="5"/>
-      <c r="B240" s="4"/>
+      <c r="A240" s="3"/>
+      <c r="B240" s="1"/>
     </row>
     <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A241" s="5"/>
-      <c r="B241" s="4"/>
+      <c r="A241" s="3"/>
+      <c r="B241" s="1"/>
     </row>
     <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="5"/>
-      <c r="B242" s="4"/>
+      <c r="A242" s="3"/>
+      <c r="B242" s="1"/>
     </row>
     <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="5"/>
-      <c r="B243" s="4"/>
+      <c r="A243" s="3"/>
+      <c r="B243" s="1"/>
     </row>
     <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A244" s="5"/>
-      <c r="B244" s="4"/>
+      <c r="A244" s="3"/>
+      <c r="B244" s="1"/>
     </row>
     <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="5"/>
-      <c r="B245" s="4"/>
+      <c r="A245" s="3"/>
+      <c r="B245" s="1"/>
     </row>
     <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A246" s="5"/>
-      <c r="B246" s="4"/>
+      <c r="A246" s="3"/>
+      <c r="B246" s="1"/>
     </row>
     <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A247" s="5"/>
-      <c r="B247" s="4"/>
+      <c r="A247" s="3"/>
+      <c r="B247" s="1"/>
     </row>
     <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="5"/>
-      <c r="B248" s="4"/>
+      <c r="A248" s="3"/>
+      <c r="B248" s="1"/>
     </row>
     <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A249" s="5"/>
-      <c r="B249" s="4"/>
+      <c r="A249" s="3"/>
+      <c r="B249" s="1"/>
     </row>
     <row r="250" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A250" s="5"/>
-      <c r="B250" s="4"/>
+      <c r="A250" s="3"/>
+      <c r="B250" s="1"/>
     </row>
     <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="5"/>
-      <c r="B251" s="4"/>
+      <c r="A251" s="3"/>
+      <c r="B251" s="1"/>
     </row>
     <row r="252" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A252" s="5"/>
-      <c r="B252" s="4"/>
+      <c r="A252" s="3"/>
+      <c r="B252" s="1"/>
     </row>
     <row r="253" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A253" s="5"/>
-      <c r="B253" s="4"/>
+      <c r="A253" s="3"/>
+      <c r="B253" s="1"/>
     </row>
     <row r="254" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A254" s="5"/>
-      <c r="B254" s="4"/>
+      <c r="A254" s="3"/>
+      <c r="B254" s="1"/>
     </row>
     <row r="255" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A255" s="5"/>
-      <c r="B255" s="4"/>
+      <c r="A255" s="3"/>
+      <c r="B255" s="1"/>
     </row>
     <row r="256" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A256" s="5"/>
-      <c r="B256" s="4"/>
+      <c r="A256" s="3"/>
+      <c r="B256" s="1"/>
     </row>
     <row r="257" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A257" s="5"/>
-      <c r="B257" s="4"/>
+      <c r="A257" s="3"/>
+      <c r="B257" s="1"/>
     </row>
     <row r="258" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A258" s="5"/>
-      <c r="B258" s="4"/>
+      <c r="A258" s="3"/>
+      <c r="B258" s="1"/>
     </row>
     <row r="259" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A259" s="5"/>
-      <c r="B259" s="4"/>
+      <c r="A259" s="3"/>
+      <c r="B259" s="1"/>
     </row>
     <row r="260" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="5"/>
-      <c r="B260" s="4"/>
+      <c r="A260" s="3"/>
+      <c r="B260" s="1"/>
     </row>
     <row r="261" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A261" s="5"/>
-      <c r="B261" s="4"/>
+      <c r="A261" s="3"/>
+      <c r="B261" s="1"/>
     </row>
     <row r="262" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="5"/>
-      <c r="B262" s="4"/>
+      <c r="A262" s="3"/>
+      <c r="B262" s="1"/>
     </row>
     <row r="263" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="5"/>
-      <c r="B263" s="4"/>
+      <c r="A263" s="3"/>
+      <c r="B263" s="1"/>
     </row>
     <row r="264" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A264" s="5"/>
-      <c r="B264" s="4"/>
+      <c r="A264" s="3"/>
+      <c r="B264" s="1"/>
     </row>
     <row r="265" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A265" s="5"/>
-      <c r="B265" s="4"/>
+      <c r="A265" s="3"/>
+      <c r="B265" s="1"/>
     </row>
     <row r="266" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A266" s="5"/>
-      <c r="B266" s="4"/>
+      <c r="A266" s="3"/>
+      <c r="B266" s="1"/>
     </row>
     <row r="267" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="5"/>
-      <c r="B267" s="4"/>
+      <c r="A267" s="3"/>
+      <c r="B267" s="1"/>
     </row>
     <row r="268" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A268" s="5"/>
-      <c r="B268" s="4"/>
+      <c r="A268" s="3"/>
+      <c r="B268" s="1"/>
     </row>
     <row r="269" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A269" s="5"/>
-      <c r="B269" s="4"/>
+      <c r="A269" s="3"/>
+      <c r="B269" s="1"/>
     </row>
     <row r="270" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A270" s="5"/>
-      <c r="B270" s="4"/>
+      <c r="A270" s="3"/>
+      <c r="B270" s="1"/>
     </row>
     <row r="271" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="272" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>